<commit_message>
update to bom. last air wires taken care of on board
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="92">
   <si>
     <t>Qty</t>
   </si>
@@ -288,6 +288,21 @@
   </si>
   <si>
     <t>package</t>
+  </si>
+  <si>
+    <t>3v linear reg</t>
+  </si>
+  <si>
+    <t>ti</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=197568672&amp;uq=635991844891259046</t>
+  </si>
+  <si>
+    <t>sot233</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/tlv1117-33.pdf</t>
   </si>
 </sst>
 </file>
@@ -633,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -964,22 +979,22 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F16">
-        <v>1.5</v>
-      </c>
-      <c r="G16" t="s">
-        <v>60</v>
+        <v>0.1</v>
+      </c>
+      <c r="G16">
+        <v>603</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -987,22 +1002,22 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" t="s">
-        <v>63</v>
+        <v>69</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F17">
-        <v>0.1</v>
-      </c>
-      <c r="G17">
-        <v>603</v>
+        <v>5.89</v>
+      </c>
+      <c r="G17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1010,59 +1025,56 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F18">
-        <v>5.89</v>
-      </c>
-      <c r="G18" t="s">
-        <v>68</v>
+        <v>1.79</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F19">
-        <v>1.79</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>85</v>
+        <v>0.1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>603</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F20">
         <v>0.1</v>
@@ -1076,16 +1088,14 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>80</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D21" s="4"/>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F21">
-        <v>0.1</v>
+        <v>0.51</v>
       </c>
       <c r="G21" s="3">
         <v>603</v>
@@ -1096,14 +1106,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F22">
-        <v>0.51</v>
+        <v>0.2</v>
       </c>
       <c r="G22" s="3">
         <v>603</v>
@@ -1114,131 +1126,157 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>91</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="E23" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F23">
-        <v>0.2</v>
-      </c>
-      <c r="G23" s="3">
-        <v>603</v>
+        <v>0.62</v>
+      </c>
+      <c r="G23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" t="s">
+        <v>3</v>
+      </c>
+      <c r="I36" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37">
+        <v>603</v>
+      </c>
+      <c r="F37" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37">
+        <v>0.44</v>
+      </c>
+      <c r="H37" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37">
         <v>2</v>
-      </c>
-      <c r="D37" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" t="s">
-        <v>1</v>
-      </c>
-      <c r="G37" t="s">
-        <v>5</v>
-      </c>
-      <c r="H37" t="s">
-        <v>3</v>
-      </c>
-      <c r="I37" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D38" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E38">
         <v>603</v>
       </c>
       <c r="F38" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G38">
-        <v>0.44</v>
+        <v>0.1</v>
       </c>
       <c r="H38" t="s">
         <v>31</v>
       </c>
       <c r="I38">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E39">
         <v>603</v>
       </c>
       <c r="F39" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G39">
-        <v>0.1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H39" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="I39">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E40">
         <v>603</v>
       </c>
       <c r="F40" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G40">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="H40" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I40">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E41">
         <v>603</v>
       </c>
       <c r="F41" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G41">
-        <v>0.16</v>
+        <v>0.1</v>
       </c>
       <c r="H41" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I41">
         <v>1</v>
@@ -1246,45 +1284,45 @@
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D42" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E42">
         <v>603</v>
       </c>
       <c r="F42" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G42">
-        <v>0.1</v>
+        <v>0.17</v>
       </c>
       <c r="H42" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D43" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E43">
         <v>603</v>
       </c>
       <c r="F43" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G43">
-        <v>0.17</v>
+        <v>0.1</v>
       </c>
       <c r="H43" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="I43">
         <v>2</v>
@@ -1292,218 +1330,195 @@
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D44" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E44">
         <v>603</v>
       </c>
       <c r="F44" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G44">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="H44" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="I44">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D45" t="s">
-        <v>54</v>
-      </c>
-      <c r="E45">
-        <v>603</v>
+        <v>59</v>
+      </c>
+      <c r="E45" t="s">
+        <v>60</v>
       </c>
       <c r="F45" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G45">
-        <v>0.12</v>
+        <v>1.5</v>
       </c>
       <c r="H45" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="I45">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D46" t="s">
-        <v>59</v>
-      </c>
-      <c r="E46" t="s">
-        <v>60</v>
+        <v>64</v>
+      </c>
+      <c r="E46">
+        <v>603</v>
       </c>
       <c r="F46" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G46">
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="H46" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="I46">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C47" t="s">
-        <v>63</v>
+      <c r="C47" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="D47" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47">
-        <v>603</v>
+        <v>67</v>
+      </c>
+      <c r="E47" t="s">
+        <v>68</v>
       </c>
       <c r="F47" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G47">
+        <v>5.89</v>
+      </c>
+      <c r="H47" t="s">
+        <v>70</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F48" t="s">
+        <v>73</v>
+      </c>
+      <c r="G48">
+        <v>1.79</v>
+      </c>
+      <c r="H48" t="s">
+        <v>74</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>75</v>
+      </c>
+      <c r="E49" s="3">
+        <v>603</v>
+      </c>
+      <c r="F49" t="s">
+        <v>76</v>
+      </c>
+      <c r="G49">
         <v>0.1</v>
       </c>
-      <c r="H47" t="s">
-        <v>31</v>
-      </c>
-      <c r="I47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C48" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D48" t="s">
-        <v>67</v>
-      </c>
-      <c r="E48" t="s">
-        <v>68</v>
-      </c>
-      <c r="F48" t="s">
-        <v>69</v>
-      </c>
-      <c r="G48">
-        <v>5.89</v>
-      </c>
-      <c r="H48" t="s">
-        <v>70</v>
-      </c>
-      <c r="I48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C49" t="s">
-        <v>71</v>
-      </c>
-      <c r="D49" t="s">
-        <v>72</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F49" t="s">
-        <v>73</v>
-      </c>
-      <c r="G49">
-        <v>1.79</v>
-      </c>
       <c r="H49" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="3:9" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D50" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E50" s="3">
         <v>603</v>
       </c>
       <c r="F50" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G50">
         <v>0.1</v>
       </c>
       <c r="H50" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D51" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E51" s="3">
         <v>603</v>
       </c>
       <c r="F51" t="s">
-        <v>79</v>
-      </c>
-      <c r="G51">
-        <v>0.1</v>
-      </c>
-      <c r="H51" t="s">
-        <v>80</v>
-      </c>
-      <c r="I51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D52" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E52" s="3">
         <v>603</v>
       </c>
       <c r="F52" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D53" t="s">
-        <v>83</v>
-      </c>
-      <c r="E53" s="3">
-        <v>603</v>
-      </c>
-      <c r="F53" t="s">
         <v>84</v>
       </c>
-      <c r="G53">
+      <c r="G52">
         <v>0.2</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H52" t="s">
         <v>70</v>
       </c>
-      <c r="I53">
+      <c r="I52">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="C48" r:id="rId2"/>
-    <hyperlink ref="C18" r:id="rId3"/>
+    <hyperlink ref="C47" r:id="rId2"/>
+    <hyperlink ref="C17" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Changed default CE trace to CE0
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>Desc.</t>
   </si>
@@ -183,14 +183,21 @@
   </si>
   <si>
     <t>25MHz ±50ppm Crystal 10pF 50 Ohm</t>
+  </si>
+  <si>
+    <t>Column9</t>
+  </si>
+  <si>
+    <t>Enough</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -257,14 +264,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -304,15 +312,26 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="3" builtinId="51"/>
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
+    <cellStyle name="Comma" xfId="5" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -359,20 +378,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B4:I23" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="B4:I23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B4:J23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B4:J23"/>
   <sortState ref="B5:I23">
     <sortCondition ref="E4:E23"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2" dataDxfId="6"/>
-    <tableColumn id="3" name="Column3" dataDxfId="5"/>
-    <tableColumn id="4" name="Column4" dataDxfId="4"/>
-    <tableColumn id="5" name="Column5" dataDxfId="3"/>
-    <tableColumn id="6" name="Column6" dataDxfId="2"/>
-    <tableColumn id="7" name="Column7" dataDxfId="1"/>
-    <tableColumn id="8" name="Column8" dataDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" name="Column2" dataDxfId="7"/>
+    <tableColumn id="3" name="Column3" dataDxfId="6"/>
+    <tableColumn id="4" name="Column4" dataDxfId="5"/>
+    <tableColumn id="5" name="Column5" dataDxfId="4"/>
+    <tableColumn id="6" name="Column6" dataDxfId="3"/>
+    <tableColumn id="7" name="Column7" dataDxfId="2"/>
+    <tableColumn id="8" name="Column8" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="9" name="Column9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -677,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -748,6 +768,9 @@
       <c r="I4" s="7" t="s">
         <v>45</v>
       </c>
+      <c r="J4" s="6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
@@ -774,6 +797,9 @@
       <c r="I5" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="J5" s="15">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B6" s="5" t="s">
@@ -800,6 +826,9 @@
       <c r="I6" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="J6" s="15" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B7" s="5" t="s">
@@ -826,6 +855,7 @@
       <c r="I7" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B8" s="5" t="s">
@@ -852,6 +882,9 @@
       <c r="I8" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="J8" s="15">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B9" s="5" t="s">
@@ -878,6 +911,9 @@
       <c r="I9" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="J9" s="15">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B10" s="8">
@@ -904,6 +940,9 @@
       <c r="I10" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="J10" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B11" s="5" t="s">
@@ -930,6 +969,7 @@
       <c r="I11" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="J11" s="15"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
@@ -956,6 +996,7 @@
       <c r="I12" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="J12" s="15"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
@@ -982,6 +1023,7 @@
       <c r="I13" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="J13" s="15"/>
       <c r="L13" t="s">
         <v>37</v>
       </c>
@@ -1011,6 +1053,9 @@
       <c r="I14" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="J14" s="16">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B15" s="5" t="s">
@@ -1037,6 +1082,7 @@
       <c r="I15" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="J15" s="15"/>
     </row>
     <row r="16" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B16" s="5" t="s">
@@ -1063,8 +1109,9 @@
       <c r="I16" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
@@ -1089,8 +1136,9 @@
       <c r="I17" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1115,8 +1163,11 @@
       <c r="I18" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="J18" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B19" s="5" t="s">
         <v>27</v>
       </c>
@@ -1141,8 +1192,11 @@
       <c r="I19" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="J19" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
@@ -1167,8 +1221,11 @@
       <c r="I20" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="J20" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1193,8 +1250,9 @@
       <c r="I21" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
@@ -1219,8 +1277,9 @@
       <c r="I22" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="J22" s="15"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B23" s="5" t="s">
         <v>9</v>
       </c>
@@ -1243,8 +1302,9 @@
         <v>7.29</v>
       </c>
       <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="J23" s="15"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C24" s="3"/>
       <c r="D24" s="11" t="s">
         <v>46</v>
@@ -1267,7 +1327,7 @@
       </c>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C25" s="3"/>
       <c r="D25" s="13" t="s">
         <v>47</v>

</xml_diff>